<commit_message>
Site atualizado para conteúdo do 3º semestre
</commit_message>
<xml_diff>
--- a/Notas.xlsx
+++ b/Notas.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Notas" sheetId="1" r:id="rId1"/>
+    <sheet name="2º semestre" sheetId="2" r:id="rId1"/>
+    <sheet name="3º semestre" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>DISCIPLINA</t>
   </si>
@@ -55,21 +56,84 @@
     <t>MF</t>
   </si>
   <si>
+    <t>FÓRMULA</t>
+  </si>
+  <si>
+    <t>SITUAÇÃO</t>
+  </si>
+  <si>
+    <t>Planilha para cálculo de notas</t>
+  </si>
+  <si>
+    <t>ANALISE DE PROC P/ SIST INFORMACAO</t>
+  </si>
+  <si>
+    <t>ENGENHARIA DE SOFTWARE I</t>
+  </si>
+  <si>
+    <t>ESTRUTURA DE DADOS II</t>
+  </si>
+  <si>
+    <t>LINGUAGEM DE PROGRAMACAO II</t>
+  </si>
+  <si>
+    <t>MATEMAT P/ SIST INFORMACAO III</t>
+  </si>
+  <si>
+    <t>SISTEMAS OPERACIONAIS</t>
+  </si>
+  <si>
+    <t>TEORIA GERAL DA ADMINISTRACAO</t>
+  </si>
+  <si>
+    <t>((A * 2 + B * 1 + C * 2 + PF * 5) / 10) + PARTIC</t>
+  </si>
+  <si>
+    <t>((A * 3 + B * 2 + PF * 5) / 10) + PARTIC</t>
+  </si>
+  <si>
+    <t>((A * 20 + B * 15 + C * 15 + PF * 50) / 100) + PARTIC</t>
+  </si>
+  <si>
+    <t>((A * 25 + B * 25 + C * 25 + D * 25 + PF * 50) / 100) + PARTIC</t>
+  </si>
+  <si>
+    <t>((A * 2 + B * 3 + PF * 5) / 10) + PARTIC</t>
+  </si>
+  <si>
+    <t>((A * 25 + B * 25 + PF * 50) / 100) + PARTIC</t>
+  </si>
+  <si>
     <t>ARQUITETURA DE COMPUTADORES</t>
   </si>
   <si>
+    <t>((A * 2 + B * 2 + C * 2 + PF * 4) / 10) + PARTIC</t>
+  </si>
+  <si>
     <t>ESTRUTURA DE DADOS I</t>
   </si>
   <si>
+    <t>((A * 3 + B * 3 + PF * 4) / 10) + PARTIC</t>
+  </si>
+  <si>
     <t>ETICA E CIDADANIA II</t>
   </si>
   <si>
+    <t>((A * 4 + B * 2 + PF * 4) / 10) + PARTIC</t>
+  </si>
+  <si>
     <t>FUNDAM SIST DE INFORMACAO II</t>
   </si>
   <si>
+    <t>((H * 3 + I * 3 + PF * 4) / 10) + PARTIC</t>
+  </si>
+  <si>
     <t>INGLES TECNICO II</t>
   </si>
   <si>
+    <t>((A * 3 + B * 3 + C * 3 + PF * 4) / 10) + PARTIC</t>
+  </si>
+  <si>
     <t>LINGUAGEM DE PROGRAMACAO I</t>
   </si>
   <si>
@@ -79,31 +143,7 @@
     <t>TECNOLOGIA WEB</t>
   </si>
   <si>
-    <t>FÓRMULA</t>
-  </si>
-  <si>
-    <t>((A * 2 + B * 2 + C * 2 + PF * 4) / 10) + PARTIC</t>
-  </si>
-  <si>
-    <t>((A * 3 + B * 3 + PF * 4) / 10) + PARTIC</t>
-  </si>
-  <si>
-    <t>((A * 4 + B * 2 + PF * 4) / 10) + PARTIC</t>
-  </si>
-  <si>
-    <t>((H * 3 + I * 3 + PF * 4) / 10) + PARTIC</t>
-  </si>
-  <si>
-    <t>((A * 3 + B * 3 + C * 3 + PF * 4) / 10) + PARTIC</t>
-  </si>
-  <si>
     <t>((A * 3 + B * 3 + C * 2 + D * 4 + PF * 8) / 20) + PARTIC</t>
-  </si>
-  <si>
-    <t>SITUAÇÃO</t>
-  </si>
-  <si>
-    <t>Planilha para cálculo de notas</t>
   </si>
 </sst>
 </file>
@@ -143,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,12 +204,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -238,32 +284,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -365,62 +385,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -429,31 +517,69 @@
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -461,11 +587,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
@@ -473,7 +639,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -831,12 +1064,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Plan1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
@@ -852,23 +1085,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
+      <c r="A1" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -911,251 +1144,251 @@
         <v>12</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="9">
+      <c r="A3" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="7">
         <f>((B3*2+C3*2+D3*2+K3*4)/10)+L3</f>
         <v>0</v>
       </c>
-      <c r="N3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="11" t="str">
+      <c r="N3" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="8" t="str">
         <f>IF(OR(B3="",C3="",D3=""),"Preencha as notas",IF(K3="",IF(M3&lt;5.5,CONCATENATE("Precisa de ", (((5.5-M3)*10)/4), " na PF"),"APROVADO SEM PF"),IF(M3&gt;=5.5,"APROVADO","REPROVADO")))</f>
         <v>Preencha as notas</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="9">
+      <c r="A4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="7">
         <f>((B4*3+C4*3+K4*4)/10)+L4</f>
         <v>0</v>
       </c>
-      <c r="N4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="11" t="str">
+      <c r="N4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="8" t="str">
         <f>IF(OR(B4="",C4=""),"Preencha as notas",IF(K4="",IF(M4&lt;5.5,CONCATENATE("Precisa de ", (((5.5-M4)*10)/4), " na PF"),"APROVADO SEM PF"),IF(M4&gt;=5.5,"APROVADO","REPROVADO")))</f>
         <v>Preencha as notas</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="9">
+      <c r="A5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="7">
         <f>((B5*4+C5*2+K5*4)/10)+L5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="11" t="str">
+      <c r="N5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="8" t="str">
         <f>IF(OR(B5="",C5=""),"Preencha as notas",IF(K5="",IF(M5&lt;5.5,CONCATENATE("Precisa de ", (((5.5-M5)*10)/4), " na PF"),"APROVADO SEM PF"),IF(M5&gt;=5.5,"APROVADO","REPROVADO")))</f>
         <v>Preencha as notas</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="9">
+      <c r="A6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="7">
         <f>((I6*3+J6*3+K6*4)/10)+L6</f>
         <v>0</v>
       </c>
-      <c r="N6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" s="11" t="str">
+      <c r="N6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="8" t="str">
         <f>IF(OR(I6="",J6=""),"Preencha as notas",IF(K6="",IF(M6&lt;5.5,CONCATENATE("Precisa de ", (((5.5-M6)*10)/4), " na PF"),"APROVADO SEM PF"),IF(M6&gt;=5.5,"APROVADO","REPROVADO")))</f>
         <v>Preencha as notas</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="9">
+      <c r="A7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="7">
         <f>((B7*3+C7*3+D7*3+K7*4)/10)+L7</f>
         <v>0</v>
       </c>
-      <c r="N7" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" s="11" t="str">
+      <c r="N7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="8" t="str">
         <f t="shared" ref="O7:O9" si="0">IF(OR(B7="",C7="",D7=""),"Preencha as notas",IF(K7="",IF(M7&lt;5.5,CONCATENATE("Precisa de ", (((5.5-M7)*10)/4), " na PF"),"APROVADO SEM PF"),IF(M7&gt;=5.5,"APROVADO","REPROVADO")))</f>
         <v>Preencha as notas</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="9">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="7">
         <f>((B8*3+C8*3+K8*4)/10)+L8</f>
         <v>0</v>
       </c>
-      <c r="N8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="11" t="str">
+      <c r="N8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="8" t="str">
         <f>IF(OR(B8="",C8=""),"Preencha as notas",IF(K8="",IF(M8&lt;5.5,CONCATENATE("Precisa de ", (((5.5-M8)*10)/4), " na PF"),"APROVADO SEM PF"),IF(M8&gt;=5.5,"APROVADO","REPROVADO")))</f>
         <v>Preencha as notas</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="9">
+      <c r="A9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="7">
         <f>((B9*2+C9*2+D9*2+K9*4)/10)+L9</f>
         <v>0</v>
       </c>
-      <c r="N9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="11" t="str">
+      <c r="N9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Preencha as notas</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="20">
+      <c r="A10" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="13">
         <f>((B10*3+C10*3+D10*2+E10*4+K10*8)/20)+L10</f>
         <v>0</v>
       </c>
-      <c r="N10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="11" t="str">
+      <c r="N10" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="8" t="str">
         <f>IF(OR(B10="",C10="",D10="",E10=""),"Preencha as notas",IF(K10="",IF(M10&lt;5.5,CONCATENATE("Precisa de ", (((5.5-M10)*10)/4), " na PF"),"APROVADO SEM PF"),IF(M10&gt;=5.5,"APROVADO","REPROVADO")))</f>
         <v>Preencha as notas</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="85E3" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="A6AD" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:M10">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThanOrEqual">
       <formula>5.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="lessThan">
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O10">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Precisa de">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Precisa de">
       <formula>NOT(ISERROR(SEARCH("Precisa de",O3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="REPROVADO">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="REPROVADO">
       <formula>NOT(ISERROR(SEARCH("REPROVADO",O3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O10">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Preencha as notas">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Preencha as notas">
       <formula>NOT(ISERROR(SEARCH("Preencha as notas",O3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1165,7 +1398,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{6B1AF9DF-3C30-456B-B365-66A805922D9E}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{52A72419-FB6B-4BAB-9DF1-5BF010BF82A0}">
             <xm:f>NOT(ISERROR(SEARCH("APROVADO",O3)))</xm:f>
             <xm:f>"APROVADO"</xm:f>
             <x14:dxf>
@@ -1185,4 +1418,358 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="6.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="60.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="7">
+        <f>((B3*2+C3*1+D3*2+K3*5)/10)+L3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="16" t="str">
+        <f>IF(OR(B3="",C3="",D3=""),"Preencha as notas",IF(K3="",IF(M3&lt;6,CONCATENATE("Precisa de ", (((6-M3)*10)/5), " na PF"),"APROVADO SEM PF"),IF(M3&gt;=6,"APROVADO","REPROVADO")))</f>
+        <v>Preencha as notas</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="27">
+        <f>L3</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <f>((B4*25+C4*25+K4*50)/100)+L4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="8" t="str">
+        <f>IF(OR(B4="",C4=""),"Preencha as notas",IF(K4="",IF(M4&lt;6,CONCATENATE("Precisa de ", (((6-M4)*10)/5), " na PF"),"APROVADO SEM PF"),IF(M4&gt;=6,"APROVADO","REPROVADO")))</f>
+        <v>Preencha as notas</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27">
+        <f t="shared" ref="L5:L9" si="0">L4</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <f>((B5*3+C5*2+K5*5)/10)+L5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="8" t="str">
+        <f>IF(OR(B5="",C5=""),"Preencha as notas",IF(K5="",IF(M5&lt;6,CONCATENATE("Precisa de ", (((6-M5)*10)/5), " na PF"),"APROVADO SEM PF"),IF(M5&gt;=6,"APROVADO","REPROVADO")))</f>
+        <v>Preencha as notas</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <f>((B6*20+C6*15+D6*15+K6*50)/100)+L6</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="8" t="str">
+        <f>IF(OR(B6="",C6="",D6=""),"Preencha as notas",IF(K6="",IF(M6&lt;6,CONCATENATE("Precisa de ", (((6-M6)*10)/5), " na PF"),"APROVADO SEM PF"),IF(M6&gt;=6,"APROVADO","REPROVADO")))</f>
+        <v>Preencha as notas</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <f>((B7*25+C7*25+D7*25+E7*25+K7*50)/100)+L7</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="8" t="str">
+        <f>IF(OR(B7="",C7="",D7="",E7=""),"Preencha as notas",IF(K7="",IF(M7&lt;6,CONCATENATE("Precisa de ", (((6-M7)*10)/5), " na PF"),"APROVADO SEM PF"),IF(M7&gt;=6,"APROVADO","REPROVADO")))</f>
+        <v>Preencha as notas</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <f>((B8*2+C8*3+K8*5)/10)+L8</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="8" t="str">
+        <f>IF(OR(B8="",C8=""),"Preencha as notas",IF(K8="",IF(M8&lt;6,CONCATENATE("Precisa de ", (((6-M8)*10)/5), " na PF"),"APROVADO SEM PF"),IF(M8&gt;=6,"APROVADO","REPROVADO")))</f>
+        <v>Preencha as notas</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13">
+        <f>((B9*2+C9*3+K9*5)/10)+L9</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="19" t="str">
+        <f>IF(OR(B9="",C9=""),"Preencha as notas",IF(K9="",IF(M9&lt;6,CONCATENATE("Precisa de ", (((6-M9)*10)/5), " na PF"),"APROVADO SEM PF"),IF(M9&gt;=6,"APROVADO","REPROVADO")))</f>
+        <v>Preencha as notas</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="AF27" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="M3:M9">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThanOrEqual">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O9">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Precisa de">
+      <formula>NOT(ISERROR(SEARCH("Precisa de",O3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="REPROVADO">
+      <formula>NOT(ISERROR(SEARCH("REPROVADO",O3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O9">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Preencha as notas">
+      <formula>NOT(ISERROR(SEARCH("Preencha as notas",O3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:L9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>OR(ISNUMBER(SEARCH("("&amp;B$2,$N3)),ISNUMBER(SEARCH("+ "&amp;B$2,$N3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{68404806-95EB-45F1-9D18-60243DAAC68B}">
+            <xm:f>NOT(ISERROR(SEARCH("APROVADO",O3)))</xm:f>
+            <xm:f>"APROVADO"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>O3:O9</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>